<commit_message>
ajustes para simplificar codigo
</commit_message>
<xml_diff>
--- a/dados/Exercicio_estimativa_de_paginas_2019_2020_joas_novo.xlsx
+++ b/dados/Exercicio_estimativa_de_paginas_2019_2020_joas_novo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wpessoa/repositorios/Fluxo_Editorial/dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C8F52A-7908-284B-9DA4-42927464D6B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4869808D-BE5B-614B-9092-9B3047EFA563}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37720" yWindow="1480" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{65A40DB1-9662-402A-9A88-8271FB79FF7C}"/>
+    <workbookView xWindow="3460" yWindow="580" windowWidth="29040" windowHeight="16440" xr2:uid="{65A40DB1-9662-402A-9A88-8271FB79FF7C}"/>
   </bookViews>
   <sheets>
     <sheet name="EXECUTADO 2019" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3705" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3713" uniqueCount="650">
   <si>
     <t>ENTIDADE</t>
   </si>
@@ -1974,6 +1974,18 @@
   </si>
   <si>
     <t>NF 1366</t>
+  </si>
+  <si>
+    <t>Diferança</t>
+  </si>
+  <si>
+    <t>Soma Quadrado</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
+  </si>
+  <si>
+    <t>RMSE Editorar</t>
   </si>
 </sst>
 </file>
@@ -1986,7 +1998,7 @@
     <numFmt numFmtId="166" formatCode="&quot;R$ &quot;#,##0.00_);\(&quot;R$ &quot;#,##0.00\)"/>
     <numFmt numFmtId="167" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2052,8 +2064,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2120,8 +2139,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF95B3D7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -2365,13 +2396,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="218">
+  <cellXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3020,6 +3064,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="11" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda 2" xfId="2" xr:uid="{CE53C7A1-FD52-450C-AB02-8D3EDFA83129}"/>
@@ -3382,10 +3445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B51CFDF2-E479-4AF3-B196-4948E99A1239}">
-  <dimension ref="A1:V78"/>
+  <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="W73" sqref="W73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3412,7 +3475,7 @@
     <col min="22" max="22" width="109.1640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="159" t="s">
         <v>0</v>
       </c>
@@ -3479,8 +3542,11 @@
       <c r="V1" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W1" s="218" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="189" t="s">
         <v>19</v>
       </c>
@@ -3550,8 +3616,12 @@
       <c r="V2" s="152" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W2" s="219">
+        <f>IF(COUNTA(S2)=1,D2-S2,"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="189" t="s">
         <v>19</v>
       </c>
@@ -3621,8 +3691,12 @@
       <c r="V3" s="153" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W3" s="219">
+        <f t="shared" ref="W3:W66" si="6">IF(COUNTA(S3)=1,D3-S3,"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="189" t="s">
         <v>19</v>
       </c>
@@ -3692,8 +3766,12 @@
       <c r="V4" s="153" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W4" s="219">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="189" t="s">
         <v>19</v>
       </c>
@@ -3763,8 +3841,12 @@
       <c r="V5" s="153" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W5" s="219">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="189" t="s">
         <v>19</v>
       </c>
@@ -3834,8 +3916,12 @@
       <c r="V6" s="153" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W6" s="219">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="189" t="s">
         <v>187</v>
       </c>
@@ -3905,8 +3991,12 @@
       <c r="V7" s="153" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W7" s="219">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="189" t="s">
         <v>19</v>
       </c>
@@ -3920,7 +4010,7 @@
         <v>66</v>
       </c>
       <c r="E8" s="169">
-        <f t="shared" ref="E8:E10" si="6">SUM(D8-C8)/C8*100%</f>
+        <f t="shared" ref="E8:E10" si="7">SUM(D8-C8)/C8*100%</f>
         <v>0.43478260869565216</v>
       </c>
       <c r="F8" s="170" t="s">
@@ -3976,8 +4066,12 @@
       <c r="V8" s="153" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W8" s="219">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="189" t="s">
         <v>19</v>
       </c>
@@ -3991,7 +4085,7 @@
         <v>102</v>
       </c>
       <c r="E9" s="169">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.54545454545454541</v>
       </c>
       <c r="F9" s="170" t="s">
@@ -4047,8 +4141,12 @@
       <c r="V9" s="153" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W9" s="219">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="189" t="s">
         <v>19</v>
       </c>
@@ -4062,7 +4160,7 @@
         <v>98</v>
       </c>
       <c r="E10" s="190">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1304347826086956</v>
       </c>
       <c r="F10" s="170" t="s">
@@ -4118,8 +4216,12 @@
       <c r="V10" s="153" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W10" s="219">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="189" t="s">
         <v>19</v>
       </c>
@@ -4189,8 +4291,12 @@
       <c r="V11" s="153" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W11" s="219">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="189" t="s">
         <v>19</v>
       </c>
@@ -4260,8 +4366,12 @@
       <c r="V12" s="153" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W12" s="219">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="189" t="s">
         <v>19</v>
       </c>
@@ -4331,8 +4441,12 @@
       <c r="V13" s="153" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W13" s="219">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="189" t="s">
         <v>187</v>
       </c>
@@ -4402,8 +4516,12 @@
       <c r="V14" s="153" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W14" s="219">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="189" t="s">
         <v>19</v>
       </c>
@@ -4473,8 +4591,12 @@
       <c r="V15" s="153" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W15" s="219">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="189" t="s">
         <v>19</v>
       </c>
@@ -4488,7 +4610,7 @@
         <v>48</v>
       </c>
       <c r="E16" s="169">
-        <f t="shared" ref="E16:E36" si="7">SUM(D16-C16)/C16*100%</f>
+        <f t="shared" ref="E16:E36" si="8">SUM(D16-C16)/C16*100%</f>
         <v>0.41176470588235292</v>
       </c>
       <c r="F16" s="170" t="s">
@@ -4544,8 +4666,12 @@
       <c r="V16" s="153" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W16" s="219">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="189" t="s">
         <v>19</v>
       </c>
@@ -4559,7 +4685,7 @@
         <v>88</v>
       </c>
       <c r="E17" s="169">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.54385964912280704</v>
       </c>
       <c r="F17" s="170" t="s">
@@ -4615,8 +4741,12 @@
       <c r="V17" s="154" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="18" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W17" s="219">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="189" t="s">
         <v>19</v>
       </c>
@@ -4630,7 +4760,7 @@
         <v>46</v>
       </c>
       <c r="E18" s="190">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0909090909090908</v>
       </c>
       <c r="F18" s="170" t="s">
@@ -4686,8 +4816,12 @@
       <c r="V18" s="153" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="19" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W18" s="219">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="189" t="s">
         <v>19</v>
       </c>
@@ -4701,7 +4835,7 @@
         <v>45</v>
       </c>
       <c r="E19" s="190">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.5</v>
       </c>
       <c r="F19" s="170" t="s">
@@ -4757,8 +4891,12 @@
       <c r="V19" s="153" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="20" spans="1:22" ht="32" x14ac:dyDescent="0.2">
+      <c r="W19" s="219">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="189" t="s">
         <v>19</v>
       </c>
@@ -4772,7 +4910,7 @@
         <v>120</v>
       </c>
       <c r="E20" s="169">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.53846153846153844</v>
       </c>
       <c r="F20" s="170" t="s">
@@ -4828,8 +4966,12 @@
       <c r="V20" s="155" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W20" s="219">
+        <f t="shared" si="6"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="189" t="s">
         <v>19</v>
       </c>
@@ -4843,7 +4985,7 @@
         <v>90</v>
       </c>
       <c r="E21" s="169">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.8</v>
       </c>
       <c r="F21" s="170" t="s">
@@ -4899,8 +5041,12 @@
       <c r="V21" s="156" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="22" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W21" s="219">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="189" t="s">
         <v>187</v>
       </c>
@@ -4914,7 +5060,7 @@
         <v>92</v>
       </c>
       <c r="E22" s="190">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4210526315789473</v>
       </c>
       <c r="F22" s="170" t="s">
@@ -4970,8 +5116,12 @@
       <c r="V22" s="153" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="23" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W22" s="219">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="189" t="s">
         <v>19</v>
       </c>
@@ -4985,7 +5135,7 @@
         <v>94</v>
       </c>
       <c r="E23" s="169">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.7407407407407407</v>
       </c>
       <c r="F23" s="170" t="s">
@@ -5041,8 +5191,12 @@
       <c r="V23" s="153" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" ht="32" x14ac:dyDescent="0.2">
+      <c r="W23" s="219">
+        <f t="shared" si="6"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="189" t="s">
         <v>19</v>
       </c>
@@ -5056,7 +5210,7 @@
         <v>130</v>
       </c>
       <c r="E24" s="169">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.47727272727272729</v>
       </c>
       <c r="F24" s="170" t="s">
@@ -5112,8 +5266,12 @@
       <c r="V24" s="153" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="25" spans="1:22" ht="48" x14ac:dyDescent="0.2">
+      <c r="W24" s="219">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="189" t="s">
         <v>19</v>
       </c>
@@ -5127,7 +5285,7 @@
         <v>134</v>
       </c>
       <c r="E25" s="169">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.47252747252747251</v>
       </c>
       <c r="F25" s="170" t="s">
@@ -5183,8 +5341,12 @@
       <c r="V25" s="153" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="26" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W25" s="219">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="189" t="s">
         <v>19</v>
       </c>
@@ -5198,7 +5360,7 @@
         <v>56</v>
       </c>
       <c r="E26" s="169">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.47368421052631576</v>
       </c>
       <c r="F26" s="170" t="s">
@@ -5254,8 +5416,12 @@
       <c r="V26" s="153" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="27" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W26" s="219">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="189" t="s">
         <v>19</v>
       </c>
@@ -5269,7 +5435,7 @@
         <v>120</v>
       </c>
       <c r="E27" s="169">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="F27" s="170" t="s">
@@ -5325,8 +5491,12 @@
       <c r="V27" s="153" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="28" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W27" s="219">
+        <f t="shared" si="6"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="189" t="s">
         <v>19</v>
       </c>
@@ -5340,7 +5510,7 @@
         <v>420</v>
       </c>
       <c r="E28" s="169">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.96261682242990654</v>
       </c>
       <c r="F28" s="170" t="s">
@@ -5396,8 +5566,12 @@
       <c r="V28" s="157" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="29" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W28" s="219">
+        <f t="shared" si="6"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="189" t="s">
         <v>19</v>
       </c>
@@ -5411,7 +5585,7 @@
         <v>48</v>
       </c>
       <c r="E29" s="190">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.1818181818181819</v>
       </c>
       <c r="F29" s="170" t="s">
@@ -5467,8 +5641,12 @@
       <c r="V29" s="157" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="30" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W29" s="219">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="189" t="s">
         <v>19</v>
       </c>
@@ -5482,7 +5660,7 @@
         <v>65</v>
       </c>
       <c r="E30" s="190">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.5</v>
       </c>
       <c r="F30" s="170" t="s">
@@ -5538,8 +5716,12 @@
       <c r="V30" s="157" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="31" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W30" s="219">
+        <f t="shared" si="6"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="189" t="s">
         <v>19</v>
       </c>
@@ -5553,7 +5735,7 @@
         <v>75</v>
       </c>
       <c r="E31" s="169">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.97368421052631582</v>
       </c>
       <c r="F31" s="170" t="s">
@@ -5609,8 +5791,12 @@
       <c r="V31" s="153" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="32" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W31" s="219">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="189" t="s">
         <v>187</v>
       </c>
@@ -5624,7 +5810,7 @@
         <v>120</v>
       </c>
       <c r="E32" s="169">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.44578313253012047</v>
       </c>
       <c r="F32" s="170" t="s">
@@ -5680,8 +5866,12 @@
       <c r="V32" s="153" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="33" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W32" s="219">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="189" t="s">
         <v>19</v>
       </c>
@@ -5695,7 +5885,7 @@
         <v>120</v>
       </c>
       <c r="E33" s="169">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="F33" s="170" t="s">
@@ -5751,8 +5941,12 @@
       <c r="V33" s="153" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="34" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W33" s="219">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="189" t="s">
         <v>19</v>
       </c>
@@ -5766,7 +5960,7 @@
         <v>75</v>
       </c>
       <c r="E34" s="169">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.875</v>
       </c>
       <c r="F34" s="170" t="s">
@@ -5822,8 +6016,12 @@
       <c r="V34" s="153" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="35" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W34" s="219">
+        <f t="shared" si="6"/>
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="189" t="s">
         <v>187</v>
       </c>
@@ -5837,7 +6035,7 @@
         <v>71</v>
       </c>
       <c r="E35" s="169">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F35" s="170" t="s">
@@ -5893,8 +6091,12 @@
       <c r="V35" s="153" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="36" spans="1:22" ht="32" x14ac:dyDescent="0.2">
+      <c r="W35" s="219">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="189" t="s">
         <v>19</v>
       </c>
@@ -5908,7 +6110,7 @@
         <v>120</v>
       </c>
       <c r="E36" s="169">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.48148148148148145</v>
       </c>
       <c r="F36" s="170" t="s">
@@ -5964,8 +6166,12 @@
       <c r="V36" s="153" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="37" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W36" s="219">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="189" t="s">
         <v>19</v>
       </c>
@@ -6035,8 +6241,12 @@
       <c r="V37" s="153" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="38" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W37" s="219">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="189" t="s">
         <v>19</v>
       </c>
@@ -6106,8 +6316,12 @@
       <c r="V38" s="153" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="39" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W38" s="219">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="189" t="s">
         <v>19</v>
       </c>
@@ -6177,8 +6391,12 @@
       <c r="V39" s="153" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="40" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W39" s="219">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="189" t="s">
         <v>187</v>
       </c>
@@ -6192,7 +6410,7 @@
         <v>300</v>
       </c>
       <c r="E40" s="169">
-        <f t="shared" ref="E40:E42" si="8">SUM(D40-C40)/C40*100%</f>
+        <f t="shared" ref="E40:E42" si="9">SUM(D40-C40)/C40*100%</f>
         <v>0.3888888888888889</v>
       </c>
       <c r="F40" s="170" t="s">
@@ -6248,8 +6466,12 @@
       <c r="V40" s="153" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="41" spans="1:22" ht="32" x14ac:dyDescent="0.2">
+      <c r="W40" s="219">
+        <f t="shared" si="6"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="189" t="s">
         <v>19</v>
       </c>
@@ -6263,7 +6485,7 @@
         <v>98</v>
       </c>
       <c r="E41" s="169">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.55555555555555558</v>
       </c>
       <c r="F41" s="170" t="s">
@@ -6319,8 +6541,12 @@
       <c r="V41" s="153" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="42" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W41" s="219">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="189" t="s">
         <v>19</v>
       </c>
@@ -6334,7 +6560,7 @@
         <v>85</v>
       </c>
       <c r="E42" s="169">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="F42" s="170" t="s">
@@ -6390,8 +6616,12 @@
       <c r="V42" s="153" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="43" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W42" s="219">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="189" t="s">
         <v>19</v>
       </c>
@@ -6461,8 +6691,12 @@
       <c r="V43" s="153" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W43" s="219">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="189" t="s">
         <v>19</v>
       </c>
@@ -6532,8 +6766,12 @@
       <c r="V44" s="153" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="45" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W44" s="219">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="189" t="s">
         <v>19</v>
       </c>
@@ -6603,8 +6841,12 @@
       <c r="V45" s="153" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="46" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W45" s="219">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="189" t="s">
         <v>19</v>
       </c>
@@ -6674,8 +6916,12 @@
       <c r="V46" s="153" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="47" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W46" s="219">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="189" t="s">
         <v>19</v>
       </c>
@@ -6745,8 +6991,12 @@
       <c r="V47" s="153" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="48" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W47" s="219">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="189" t="s">
         <v>19</v>
       </c>
@@ -6760,7 +7010,7 @@
         <v>48</v>
       </c>
       <c r="E48" s="169">
-        <f t="shared" ref="E48:E70" si="9">SUM(D48-C48)/C48*100%</f>
+        <f t="shared" ref="E48:E70" si="10">SUM(D48-C48)/C48*100%</f>
         <v>0.65517241379310343</v>
       </c>
       <c r="F48" s="170" t="s">
@@ -6816,8 +7066,12 @@
       <c r="V48" s="153" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="49" spans="1:22" ht="32" x14ac:dyDescent="0.2">
+      <c r="W48" s="219">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="189" t="s">
         <v>19</v>
       </c>
@@ -6831,7 +7085,7 @@
         <v>88</v>
       </c>
       <c r="E49" s="169">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.51724137931034486</v>
       </c>
       <c r="F49" s="170" t="s">
@@ -6887,8 +7141,12 @@
       <c r="V49" s="153" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="50" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W49" s="219">
+        <f t="shared" si="6"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="189" t="s">
         <v>19</v>
       </c>
@@ -6902,7 +7160,7 @@
         <v>48</v>
       </c>
       <c r="E50" s="169">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.25</v>
       </c>
       <c r="F50" s="170" t="s">
@@ -6958,8 +7216,12 @@
       <c r="V50" s="153" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="51" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W50" s="219">
+        <f t="shared" si="6"/>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="189" t="s">
         <v>19</v>
       </c>
@@ -7029,8 +7291,12 @@
       <c r="V51" s="153" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="52" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W51" s="219">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="189" t="s">
         <v>19</v>
       </c>
@@ -7100,8 +7366,12 @@
       <c r="V52" s="153" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="53" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W52" s="219">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="189" t="s">
         <v>19</v>
       </c>
@@ -7171,8 +7441,12 @@
       <c r="V53" s="153" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="54" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W53" s="219">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="189" t="s">
         <v>187</v>
       </c>
@@ -7242,8 +7516,12 @@
       <c r="V54" s="153" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="55" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W54" s="219">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="189" t="s">
         <v>19</v>
       </c>
@@ -7313,8 +7591,12 @@
       <c r="V55" s="153" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="56" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W55" s="219">
+        <f t="shared" si="6"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="189" t="s">
         <v>19</v>
       </c>
@@ -7328,7 +7610,7 @@
         <v>150</v>
       </c>
       <c r="E56" s="169">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.40186915887850466</v>
       </c>
       <c r="F56" s="170" t="s">
@@ -7384,8 +7666,12 @@
       <c r="V56" s="153" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="57" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W56" s="219">
+        <f t="shared" si="6"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="189" t="s">
         <v>19</v>
       </c>
@@ -7399,7 +7685,7 @@
         <v>125</v>
       </c>
       <c r="E57" s="169">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.47058823529411764</v>
       </c>
       <c r="F57" s="170" t="s">
@@ -7455,8 +7741,12 @@
       <c r="V57" s="154" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="58" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W57" s="219">
+        <f t="shared" si="6"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="189" t="s">
         <v>19</v>
       </c>
@@ -7470,7 +7760,7 @@
         <v>95</v>
       </c>
       <c r="E58" s="169">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.41791044776119401</v>
       </c>
       <c r="F58" s="170" t="s">
@@ -7526,8 +7816,12 @@
       <c r="V58" s="153" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="59" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W58" s="219">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="189" t="s">
         <v>187</v>
       </c>
@@ -7541,7 +7835,7 @@
         <v>110</v>
       </c>
       <c r="E59" s="169">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.41025641025641024</v>
       </c>
       <c r="F59" s="170" t="s">
@@ -7597,8 +7891,12 @@
       <c r="V59" s="153" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="60" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W59" s="219">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="189" t="s">
         <v>52</v>
       </c>
@@ -7612,7 +7910,7 @@
         <v>400</v>
       </c>
       <c r="E60" s="169">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.26335174953959484</v>
       </c>
       <c r="F60" s="170" t="s">
@@ -7668,8 +7966,12 @@
       <c r="V60" s="155" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="61" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W60" s="219">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="189" t="s">
         <v>19</v>
       </c>
@@ -7683,7 +7985,7 @@
         <v>80</v>
       </c>
       <c r="E61" s="190">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.95121951219512191</v>
       </c>
       <c r="F61" s="170" t="s">
@@ -7739,8 +8041,12 @@
       <c r="V61" s="156" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="62" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W61" s="219">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="189" t="s">
         <v>19</v>
       </c>
@@ -7754,7 +8060,7 @@
         <v>44</v>
       </c>
       <c r="E62" s="169">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="F62" s="170" t="s">
@@ -7810,8 +8116,12 @@
       <c r="V62" s="153" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="63" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W62" s="219">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="189" t="s">
         <v>19</v>
       </c>
@@ -7825,7 +8135,7 @@
         <v>160</v>
       </c>
       <c r="E63" s="169">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.42857142857142855</v>
       </c>
       <c r="F63" s="170" t="s">
@@ -7881,8 +8191,12 @@
       <c r="V63" s="153" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="64" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W63" s="219">
+        <f t="shared" si="6"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="189" t="s">
         <v>19</v>
       </c>
@@ -7896,7 +8210,7 @@
         <v>70</v>
       </c>
       <c r="E64" s="169">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.55555555555555558</v>
       </c>
       <c r="F64" s="170" t="s">
@@ -7952,8 +8266,12 @@
       <c r="V64" s="153" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="65" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W64" s="219">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="189" t="s">
         <v>19</v>
       </c>
@@ -7967,7 +8285,7 @@
         <v>45</v>
       </c>
       <c r="E65" s="190">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.368421052631579</v>
       </c>
       <c r="F65" s="170" t="s">
@@ -8023,8 +8341,12 @@
       <c r="V65" s="153" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="66" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W65" s="219">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="189" t="s">
         <v>19</v>
       </c>
@@ -8038,7 +8360,7 @@
         <v>68</v>
       </c>
       <c r="E66" s="169">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.88888888888888884</v>
       </c>
       <c r="F66" s="170" t="s">
@@ -8094,8 +8416,12 @@
       <c r="V66" s="153" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="67" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W66" s="219">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="189" t="s">
         <v>19</v>
       </c>
@@ -8109,7 +8435,7 @@
         <v>80</v>
       </c>
       <c r="E67" s="169">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.56862745098039214</v>
       </c>
       <c r="F67" s="170" t="s">
@@ -8165,8 +8491,12 @@
       <c r="V67" s="153" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="68" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W67" s="219">
+        <f t="shared" ref="W67:W70" si="11">IF(COUNTA(S67)=1,D67-S67,"")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="179" t="s">
         <v>19</v>
       </c>
@@ -8236,8 +8566,12 @@
       <c r="V68" s="158" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="69" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W68" s="219">
+        <f t="shared" si="11"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="179" t="s">
         <v>19</v>
       </c>
@@ -8251,7 +8585,7 @@
         <v>40</v>
       </c>
       <c r="E69" s="188">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F69" s="181" t="s">
@@ -8301,14 +8635,18 @@
         <v>0</v>
       </c>
       <c r="U69" s="188">
-        <f t="shared" ref="U69" si="10">SUM(D69-S69)/D69*100%</f>
+        <f t="shared" ref="U69" si="12">SUM(D69-S69)/D69*100%</f>
         <v>0</v>
       </c>
       <c r="V69" s="158" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="70" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W69" s="219">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="179" t="s">
         <v>19</v>
       </c>
@@ -8322,7 +8660,7 @@
         <v>196</v>
       </c>
       <c r="E70" s="188">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F70" s="181" t="s">
@@ -8378,16 +8716,48 @@
       <c r="V70" s="158" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="73" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W70" s="219">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U71" s="222" t="s">
+        <v>647</v>
+      </c>
+      <c r="V71" s="223"/>
+      <c r="W71" s="224">
+        <f>SUMSQ(W2:W70)</f>
+        <v>51794</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U72" s="222" t="s">
+        <v>648</v>
+      </c>
+      <c r="V72" s="223"/>
+      <c r="W72" s="224">
+        <f>COUNT(W2:W70)</f>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="E73" s="66" t="s">
         <v>390</v>
       </c>
       <c r="T73" s="66" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="U73" s="225" t="s">
+        <v>649</v>
+      </c>
+      <c r="V73" s="223"/>
+      <c r="W73" s="226">
+        <f>SQRT(W71/W72)</f>
+        <v>27.397767813444588</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C74" s="217" t="s">
         <v>389</v>
       </c>
@@ -8420,7 +8790,7 @@
         <v>0.1334030966806202</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C75" s="217" t="s">
         <v>391</v>
       </c>
@@ -8449,7 +8819,7 @@
         <v>0.36922475220474349</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C76" s="217" t="s">
         <v>392</v>
       </c>
@@ -8478,7 +8848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C78" s="135"/>
       <c r="S78" s="135"/>
       <c r="T78" s="56"/>
@@ -8518,10 +8888,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B00B66-C32D-4DEF-9BC0-D9C09304FF24}">
-  <dimension ref="A1:V94"/>
+  <dimension ref="A1:W94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="U87" sqref="U87:W89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8531,16 +8901,16 @@
     <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.5" customWidth="1"/>
-    <col min="8" max="8" width="102.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="102.6640625" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
-    <col min="13" max="15" width="9" customWidth="1"/>
-    <col min="16" max="16" width="13.5" customWidth="1"/>
-    <col min="17" max="17" width="9" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" hidden="1" customWidth="1"/>
+    <col min="13" max="15" width="9" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="9" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="12.5" customWidth="1"/>
     <col min="19" max="19" width="9" customWidth="1"/>
     <col min="20" max="20" width="20.5" customWidth="1"/>
@@ -8548,7 +8918,7 @@
     <col min="22" max="22" width="109.1640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8615,8 +8985,11 @@
       <c r="V1" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W1" s="218" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="103" t="s">
         <v>19</v>
       </c>
@@ -8686,8 +9059,12 @@
       <c r="V2" s="111" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W2" s="219">
+        <f>IF(COUNTA(S2)=1,D2-S2,"")</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="103" t="s">
         <v>19</v>
       </c>
@@ -8757,8 +9134,12 @@
       <c r="V3" s="111" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W3" s="219">
+        <f t="shared" ref="W3:W66" si="3">IF(COUNTA(S3)=1,D3-S3,"")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="103" t="s">
         <v>52</v>
       </c>
@@ -8828,8 +9209,12 @@
       <c r="V4" s="111" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W4" s="219">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="103" t="s">
         <v>52</v>
       </c>
@@ -8899,8 +9284,12 @@
       <c r="V5" s="111" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W5" s="219">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="103" t="s">
         <v>52</v>
       </c>
@@ -8970,8 +9359,12 @@
       <c r="V6" s="111" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W6" s="219">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="103" t="s">
         <v>52</v>
       </c>
@@ -8985,7 +9378,7 @@
         <v>48</v>
       </c>
       <c r="E7" s="134">
-        <f t="shared" ref="E7:E35" si="3">SUM(D7-C7)/C7*100%</f>
+        <f t="shared" ref="E7:E35" si="4">SUM(D7-C7)/C7*100%</f>
         <v>1</v>
       </c>
       <c r="F7" s="105" t="s">
@@ -9041,8 +9434,12 @@
       <c r="V7" s="111" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W7" s="219">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="103" t="s">
         <v>52</v>
       </c>
@@ -9056,7 +9453,7 @@
         <v>40</v>
       </c>
       <c r="E8" s="134">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="F8" s="105" t="s">
@@ -9112,8 +9509,12 @@
       <c r="V8" s="111" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W8" s="219">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="103" t="s">
         <v>52</v>
       </c>
@@ -9127,7 +9528,7 @@
         <v>45</v>
       </c>
       <c r="E9" s="134">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0454545454545454</v>
       </c>
       <c r="F9" s="105" t="s">
@@ -9183,8 +9584,12 @@
       <c r="V9" s="111" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W9" s="219">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="103" t="s">
         <v>52</v>
       </c>
@@ -9254,8 +9659,12 @@
       <c r="V10" s="111" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W10" s="219">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="103" t="s">
         <v>52</v>
       </c>
@@ -9325,8 +9734,12 @@
       <c r="V11" s="111" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W11" s="219">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="103" t="s">
         <v>19</v>
       </c>
@@ -9396,8 +9809,12 @@
       <c r="V12" s="111" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W12" s="219">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="103" t="s">
         <v>19</v>
       </c>
@@ -9467,8 +9884,12 @@
       <c r="V13" s="111" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W13" s="219">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="103" t="s">
         <v>19</v>
       </c>
@@ -9538,8 +9959,12 @@
       <c r="V14" s="111" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W14" s="219">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="103" t="s">
         <v>19</v>
       </c>
@@ -9553,7 +9978,7 @@
         <v>45</v>
       </c>
       <c r="E15" s="134">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.368421052631579</v>
       </c>
       <c r="F15" s="105" t="s">
@@ -9609,8 +10034,12 @@
       <c r="V15" s="111" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W15" s="219">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="103" t="s">
         <v>19</v>
       </c>
@@ -9624,7 +10053,7 @@
         <v>110</v>
       </c>
       <c r="E16" s="90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.64179104477611937</v>
       </c>
       <c r="F16" s="105" t="s">
@@ -9680,8 +10109,12 @@
       <c r="V16" s="116" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W16" s="219">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="103" t="s">
         <v>19</v>
       </c>
@@ -9695,7 +10128,7 @@
         <v>75</v>
       </c>
       <c r="E17" s="134">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.97368421052631582</v>
       </c>
       <c r="F17" s="105" t="s">
@@ -9751,8 +10184,12 @@
       <c r="V17" s="111" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="18" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W17" s="219">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="103" t="s">
         <v>19</v>
       </c>
@@ -9766,7 +10203,7 @@
         <v>310</v>
       </c>
       <c r="E18" s="90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.49758454106280192</v>
       </c>
       <c r="F18" s="105" t="s">
@@ -9822,8 +10259,12 @@
       <c r="V18" s="111" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="19" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W18" s="219">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="117" t="s">
         <v>19</v>
       </c>
@@ -9837,7 +10278,7 @@
         <v>80</v>
       </c>
       <c r="E19" s="90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.73913043478260865</v>
       </c>
       <c r="F19" s="118" t="s">
@@ -9893,8 +10334,12 @@
       <c r="V19" s="126" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="20" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W19" s="219">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="91" t="s">
         <v>19</v>
       </c>
@@ -9908,7 +10353,7 @@
         <v>100</v>
       </c>
       <c r="E20" s="90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.4925373134328358</v>
       </c>
       <c r="F20" s="94" t="s">
@@ -9964,8 +10409,12 @@
       <c r="V20" s="127" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W20" s="219">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="103" t="s">
         <v>19</v>
       </c>
@@ -9979,7 +10428,7 @@
         <v>15</v>
       </c>
       <c r="E21" s="90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F21" s="105" t="s">
@@ -10035,8 +10484,12 @@
       <c r="V21" s="111" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="22" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W21" s="219">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="103" t="s">
         <v>19</v>
       </c>
@@ -10050,7 +10503,7 @@
         <v>72</v>
       </c>
       <c r="E22" s="90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.67441860465116277</v>
       </c>
       <c r="F22" s="105" t="s">
@@ -10106,8 +10559,12 @@
       <c r="V22" s="111" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="23" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W22" s="219">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="103" t="s">
         <v>187</v>
       </c>
@@ -10121,7 +10578,7 @@
         <v>120</v>
       </c>
       <c r="E23" s="90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.53846153846153844</v>
       </c>
       <c r="F23" s="105" t="s">
@@ -10177,8 +10634,12 @@
       <c r="V23" s="111" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W23" s="219">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="103" t="s">
         <v>52</v>
       </c>
@@ -10192,7 +10653,7 @@
         <v>120</v>
       </c>
       <c r="E24" s="90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="F24" s="105" t="s">
@@ -10248,8 +10709,12 @@
       <c r="V24" s="111" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="25" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W24" s="219">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="103" t="s">
         <v>19</v>
       </c>
@@ -10263,7 +10728,7 @@
         <v>40</v>
       </c>
       <c r="E25" s="134">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3529411764705883</v>
       </c>
       <c r="F25" s="105" t="s">
@@ -10319,8 +10784,12 @@
       <c r="V25" s="111" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="26" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W25" s="219">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="103" t="s">
         <v>19</v>
       </c>
@@ -10334,7 +10803,7 @@
         <v>80</v>
       </c>
       <c r="E26" s="90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
       <c r="F26" s="105" t="s">
@@ -10390,8 +10859,12 @@
       <c r="V26" s="111" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="27" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W26" s="219">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="103" t="s">
         <v>187</v>
       </c>
@@ -10405,7 +10878,7 @@
         <v>71</v>
       </c>
       <c r="E27" s="90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.29090909090909089</v>
       </c>
       <c r="F27" s="105" t="s">
@@ -10461,8 +10934,12 @@
       <c r="V27" s="128" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="28" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W27" s="219">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="132" t="s">
         <v>52</v>
       </c>
@@ -10476,7 +10953,7 @@
         <v>71</v>
       </c>
       <c r="E28" s="90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.29090909090909089</v>
       </c>
       <c r="F28" s="105" t="s">
@@ -10532,8 +11009,12 @@
       <c r="V28" s="128" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="29" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W28" s="219">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="132" t="s">
         <v>227</v>
       </c>
@@ -10547,7 +11028,7 @@
         <v>71</v>
       </c>
       <c r="E29" s="90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.29090909090909089</v>
       </c>
       <c r="F29" s="105" t="s">
@@ -10603,8 +11084,12 @@
       <c r="V29" s="128" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="30" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W29" s="219">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="103" t="s">
         <v>19</v>
       </c>
@@ -10618,7 +11103,7 @@
         <v>130</v>
       </c>
       <c r="E30" s="90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.51162790697674421</v>
       </c>
       <c r="F30" s="105" t="s">
@@ -10674,8 +11159,12 @@
       <c r="V30" s="111" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="31" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W30" s="219">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="103" t="s">
         <v>19</v>
       </c>
@@ -10689,7 +11178,7 @@
         <v>135</v>
       </c>
       <c r="E31" s="90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="F31" s="105" t="s">
@@ -10745,8 +11234,12 @@
       <c r="V31" s="111" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="32" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W31" s="219">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="103" t="s">
         <v>19</v>
       </c>
@@ -10760,7 +11253,7 @@
         <v>84</v>
       </c>
       <c r="E32" s="90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="F32" s="105" t="s">
@@ -10816,8 +11309,12 @@
       <c r="V32" s="111" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="33" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W32" s="219">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="103" t="s">
         <v>52</v>
       </c>
@@ -10831,7 +11328,7 @@
         <v>168</v>
       </c>
       <c r="E33" s="90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F33" s="105" t="s">
@@ -10887,8 +11384,12 @@
       <c r="V33" s="111" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="34" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W33" s="219">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="103" t="s">
         <v>187</v>
       </c>
@@ -10902,7 +11403,7 @@
         <v>162</v>
       </c>
       <c r="E34" s="90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F34" s="105" t="s">
@@ -10958,8 +11459,12 @@
       <c r="V34" s="111" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="35" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W34" s="219">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="103" t="s">
         <v>19</v>
       </c>
@@ -10973,7 +11478,7 @@
         <v>70</v>
       </c>
       <c r="E35" s="90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.52173913043478259</v>
       </c>
       <c r="F35" s="105" t="s">
@@ -11029,8 +11534,12 @@
       <c r="V35" s="111" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="36" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W35" s="219">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="103" t="s">
         <v>19</v>
       </c>
@@ -11100,8 +11609,12 @@
       <c r="V36" s="111" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="37" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W36" s="219">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="103" t="s">
         <v>19</v>
       </c>
@@ -11171,8 +11684,12 @@
       <c r="V37" s="111" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="38" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W37" s="219">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="103" t="s">
         <v>19</v>
       </c>
@@ -11242,8 +11759,12 @@
       <c r="V38" s="111" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="39" spans="1:22" ht="32" x14ac:dyDescent="0.2">
+      <c r="W38" s="219">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="103" t="s">
         <v>19</v>
       </c>
@@ -11257,7 +11778,7 @@
         <v>48</v>
       </c>
       <c r="E39" s="134">
-        <f t="shared" ref="E39:E40" si="4">SUM(D39-C39)/C39*100%</f>
+        <f t="shared" ref="E39:E40" si="5">SUM(D39-C39)/C39*100%</f>
         <v>1.4</v>
       </c>
       <c r="F39" s="105" t="s">
@@ -11313,8 +11834,12 @@
       <c r="V39" s="111" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="40" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="W39" s="219">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="103" t="s">
         <v>19</v>
       </c>
@@ -11328,7 +11853,7 @@
         <v>90</v>
       </c>
       <c r="E40" s="90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.52542372881355937</v>
       </c>
       <c r="F40" s="105" t="s">
@@ -11384,8 +11909,12 @@
       <c r="V40" s="111" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="41" spans="1:22" s="208" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="W40" s="219">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" s="208" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="192" t="s">
         <v>19</v>
       </c>
@@ -11455,8 +11984,12 @@
       <c r="V41" s="202" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="42" spans="1:22" s="208" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="W41" s="219">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" s="208" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="192" t="s">
         <v>19</v>
       </c>
@@ -11470,7 +12003,7 @@
         <v>34</v>
       </c>
       <c r="E42" s="195">
-        <f t="shared" ref="E42:E86" si="5">SUM(D42-C42)/C42*100%</f>
+        <f t="shared" ref="E42:E86" si="6">SUM(D42-C42)/C42*100%</f>
         <v>0.7142857142857143</v>
       </c>
       <c r="F42" s="196" t="s">
@@ -11516,15 +12049,19 @@
         <v>136</v>
       </c>
       <c r="T42" s="195">
-        <f t="shared" ref="T42:T47" si="6">SUM(S42-C42)/C42*100%</f>
+        <f t="shared" ref="T42:T47" si="7">SUM(S42-C42)/C42*100%</f>
         <v>0.35714285714285715</v>
       </c>
       <c r="U42" s="195">
-        <f t="shared" ref="U42:U47" si="7">SUM(D42-S42)/D42*100%</f>
+        <f t="shared" ref="U42:U47" si="8">SUM(D42-S42)/D42*100%</f>
         <v>0.20833333333333334</v>
       </c>
-    </row>
-    <row r="43" spans="1:22" s="208" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="W42" s="219">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" s="208" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="192" t="s">
         <v>19</v>
       </c>
@@ -11538,7 +12075,7 @@
         <v>34</v>
       </c>
       <c r="E43" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.65517241379310343</v>
       </c>
       <c r="F43" s="196" t="s">
@@ -11584,15 +12121,19 @@
         <v>470</v>
       </c>
       <c r="T43" s="195">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.37931034482758619</v>
       </c>
       <c r="U43" s="195">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.16666666666666666</v>
       </c>
-    </row>
-    <row r="44" spans="1:22" s="208" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="W43" s="219">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" s="208" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="192" t="s">
         <v>19</v>
       </c>
@@ -11606,7 +12147,7 @@
         <v>494</v>
       </c>
       <c r="E44" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.5625</v>
       </c>
       <c r="F44" s="196" t="s">
@@ -11652,15 +12193,19 @@
         <v>50</v>
       </c>
       <c r="T44" s="195">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.375</v>
       </c>
       <c r="U44" s="195">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.12</v>
       </c>
-    </row>
-    <row r="45" spans="1:22" s="208" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W44" s="219">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" s="208" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="192" t="s">
         <v>19</v>
       </c>
@@ -11674,7 +12219,7 @@
         <v>65</v>
       </c>
       <c r="E45" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.74358974358974361</v>
       </c>
       <c r="F45" s="196" t="s">
@@ -11720,15 +12265,19 @@
         <v>34</v>
       </c>
       <c r="T45" s="195">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.23076923076923078</v>
       </c>
       <c r="U45" s="195">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.29411764705882354</v>
       </c>
-    </row>
-    <row r="46" spans="1:22" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W45" s="219">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="192" t="s">
         <v>19</v>
       </c>
@@ -11742,7 +12291,7 @@
         <v>467</v>
       </c>
       <c r="E46" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="F46" s="196" t="s">
@@ -11788,15 +12337,19 @@
         <v>292</v>
       </c>
       <c r="T46" s="195">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="U46" s="195">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.22857142857142856</v>
       </c>
-    </row>
-    <row r="47" spans="1:22" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W46" s="219">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="192" t="s">
         <v>19</v>
       </c>
@@ -11810,7 +12363,7 @@
         <v>34</v>
       </c>
       <c r="E47" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="F47" s="196" t="s">
@@ -11856,15 +12409,19 @@
         <v>499</v>
       </c>
       <c r="T47" s="195">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.375</v>
       </c>
       <c r="U47" s="195">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8.3333333333333329E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:22" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W47" s="219">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="192" t="s">
         <v>19</v>
       </c>
@@ -11878,7 +12435,7 @@
         <v>467</v>
       </c>
       <c r="E48" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.75</v>
       </c>
       <c r="F48" s="196" t="s">
@@ -11924,15 +12481,19 @@
         <v>502</v>
       </c>
       <c r="T48" s="195">
-        <f t="shared" ref="T48:T86" si="8">SUM(S48-C48)/C48*100%</f>
+        <f t="shared" ref="T48:T86" si="9">SUM(S48-C48)/C48*100%</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="U48" s="195">
-        <f t="shared" ref="U48:U86" si="9">SUM(D48-S48)/D48*100%</f>
+        <f t="shared" ref="U48:U86" si="10">SUM(D48-S48)/D48*100%</f>
         <v>0.11428571428571428</v>
       </c>
-    </row>
-    <row r="49" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W48" s="219">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="192" t="s">
         <v>19</v>
       </c>
@@ -11946,7 +12507,7 @@
         <v>65</v>
       </c>
       <c r="E49" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.74358974358974361</v>
       </c>
       <c r="F49" s="196" t="s">
@@ -11992,15 +12553,19 @@
         <v>50</v>
       </c>
       <c r="T49" s="195">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.69230769230769229</v>
       </c>
       <c r="U49" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.9411764705882353E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W49" s="219">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="192" t="s">
         <v>19</v>
       </c>
@@ -12014,7 +12579,7 @@
         <v>473</v>
       </c>
       <c r="E50" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.50684931506849318</v>
       </c>
       <c r="F50" s="196" t="s">
@@ -12060,15 +12625,19 @@
         <v>473</v>
       </c>
       <c r="T50" s="195">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.50684931506849318</v>
       </c>
       <c r="U50" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W50" s="219">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="192" t="s">
         <v>19</v>
       </c>
@@ -12082,7 +12651,7 @@
         <v>508</v>
       </c>
       <c r="E51" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.40625</v>
       </c>
       <c r="F51" s="196" t="s">
@@ -12126,11 +12695,15 @@
         <v>-1</v>
       </c>
       <c r="U51" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W51" s="219" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="192" t="s">
         <v>19</v>
       </c>
@@ -12144,7 +12717,7 @@
         <v>34</v>
       </c>
       <c r="E52" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0869565217391304</v>
       </c>
       <c r="F52" s="196" t="s">
@@ -12190,15 +12763,19 @@
         <v>80</v>
       </c>
       <c r="T52" s="195">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.30434782608695654</v>
       </c>
       <c r="U52" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.375</v>
       </c>
-    </row>
-    <row r="53" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W52" s="219">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="192" t="s">
         <v>19</v>
       </c>
@@ -12212,7 +12789,7 @@
         <v>65</v>
       </c>
       <c r="E53" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="F53" s="196" t="s">
@@ -12258,15 +12835,19 @@
         <v>499</v>
       </c>
       <c r="T53" s="195">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.29411764705882354</v>
       </c>
       <c r="U53" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.35294117647058826</v>
       </c>
-    </row>
-    <row r="54" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W53" s="219">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="192" t="s">
         <v>19</v>
       </c>
@@ -12280,7 +12861,7 @@
         <v>34</v>
       </c>
       <c r="E54" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.1818181818181819</v>
       </c>
       <c r="F54" s="196" t="s">
@@ -12326,15 +12907,19 @@
         <v>80</v>
       </c>
       <c r="T54" s="195">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="U54" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.375</v>
       </c>
-    </row>
-    <row r="55" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W54" s="219">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="192" t="s">
         <v>19</v>
       </c>
@@ -12348,7 +12933,7 @@
         <v>34</v>
       </c>
       <c r="E55" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="F55" s="196" t="s">
@@ -12394,15 +12979,19 @@
         <v>482</v>
       </c>
       <c r="T55" s="195">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="U55" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.125</v>
       </c>
-    </row>
-    <row r="56" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W55" s="219">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="192" t="s">
         <v>19</v>
       </c>
@@ -12416,7 +13005,7 @@
         <v>34</v>
       </c>
       <c r="E56" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.41176470588235292</v>
       </c>
       <c r="F56" s="196" t="s">
@@ -12454,15 +13043,19 @@
       <c r="R56" s="201"/>
       <c r="S56" s="12"/>
       <c r="T56" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U56" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W56" s="219" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="192" t="s">
         <v>19</v>
       </c>
@@ -12476,7 +13069,7 @@
         <v>34</v>
       </c>
       <c r="E57" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="F57" s="196" t="s">
@@ -12516,15 +13109,19 @@
       <c r="R57" s="201"/>
       <c r="S57" s="12"/>
       <c r="T57" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U57" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W57" s="219" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="192" t="s">
         <v>19</v>
       </c>
@@ -12538,7 +13135,7 @@
         <v>34</v>
       </c>
       <c r="E58" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.6</v>
       </c>
       <c r="F58" s="196" t="s">
@@ -12578,15 +13175,19 @@
       <c r="R58" s="201"/>
       <c r="S58" s="12"/>
       <c r="T58" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U58" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W58" s="219" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="192" t="s">
         <v>19</v>
       </c>
@@ -12600,7 +13201,7 @@
         <v>124</v>
       </c>
       <c r="E59" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.44117647058823528</v>
       </c>
       <c r="F59" s="196" t="s">
@@ -12640,15 +13241,19 @@
       <c r="R59" s="201"/>
       <c r="S59" s="12"/>
       <c r="T59" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U59" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W59" s="219" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="192" t="s">
         <v>19</v>
       </c>
@@ -12662,7 +13267,7 @@
         <v>34</v>
       </c>
       <c r="E60" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.84615384615384615</v>
       </c>
       <c r="F60" s="196" t="s">
@@ -12702,15 +13307,19 @@
       <c r="R60" s="201"/>
       <c r="S60" s="12"/>
       <c r="T60" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U60" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W60" s="219" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="192" t="s">
         <v>19</v>
       </c>
@@ -12724,7 +13333,7 @@
         <v>73</v>
       </c>
       <c r="E61" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="F61" s="196" t="s">
@@ -12764,15 +13373,19 @@
       <c r="R61" s="201"/>
       <c r="S61" s="12"/>
       <c r="T61" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U61" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W61" s="219" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="192" t="s">
         <v>19</v>
       </c>
@@ -12786,7 +13399,7 @@
         <v>73</v>
       </c>
       <c r="E62" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0909090909090908</v>
       </c>
       <c r="F62" s="196" t="s">
@@ -12826,15 +13439,19 @@
       <c r="R62" s="201"/>
       <c r="S62" s="12"/>
       <c r="T62" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U62" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W62" s="219" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="192" t="s">
         <v>19</v>
       </c>
@@ -12848,7 +13465,7 @@
         <v>73</v>
       </c>
       <c r="E63" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.3</v>
       </c>
       <c r="F63" s="196" t="s">
@@ -12888,15 +13505,19 @@
       <c r="R63" s="201"/>
       <c r="S63" s="12"/>
       <c r="T63" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U63" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W63" s="219" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="192" t="s">
         <v>19</v>
       </c>
@@ -12910,7 +13531,7 @@
         <v>576</v>
       </c>
       <c r="E64" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.39436619718309857</v>
       </c>
       <c r="F64" s="196" t="s">
@@ -12950,15 +13571,19 @@
       <c r="R64" s="201"/>
       <c r="S64" s="12"/>
       <c r="T64" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U64" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:22" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W64" s="219" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="192" t="s">
         <v>19</v>
       </c>
@@ -12972,7 +13597,7 @@
         <v>473</v>
       </c>
       <c r="E65" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.46666666666666667</v>
       </c>
       <c r="F65" s="196" t="s">
@@ -13010,15 +13635,19 @@
       <c r="R65" s="201"/>
       <c r="S65" s="12"/>
       <c r="T65" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U65" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:22" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W65" s="219" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="192" t="s">
         <v>19</v>
       </c>
@@ -13032,7 +13661,7 @@
         <v>65</v>
       </c>
       <c r="E66" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.78947368421052633</v>
       </c>
       <c r="F66" s="196" t="s">
@@ -13070,15 +13699,19 @@
       <c r="R66" s="201"/>
       <c r="S66" s="12"/>
       <c r="T66" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U66" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:22" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W66" s="219" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="192" t="s">
         <v>19</v>
       </c>
@@ -13092,7 +13725,7 @@
         <v>494</v>
       </c>
       <c r="E67" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.5625</v>
       </c>
       <c r="F67" s="196" t="s">
@@ -13130,15 +13763,19 @@
       <c r="R67" s="201"/>
       <c r="S67" s="12"/>
       <c r="T67" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U67" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:22" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W67" s="219" t="str">
+        <f t="shared" ref="W67:W86" si="11">IF(COUNTA(S67)=1,D67-S67,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="192" t="s">
         <v>187</v>
       </c>
@@ -13152,7 +13789,7 @@
         <v>467</v>
       </c>
       <c r="E68" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.55555555555555558</v>
       </c>
       <c r="F68" s="196" t="s">
@@ -13188,15 +13825,19 @@
       <c r="R68" s="201"/>
       <c r="S68" s="12"/>
       <c r="T68" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U68" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:22" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W68" s="219" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="192" t="s">
         <v>187</v>
       </c>
@@ -13210,7 +13851,7 @@
         <v>595</v>
       </c>
       <c r="E69" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.40740740740740738</v>
       </c>
       <c r="F69" s="196" t="s">
@@ -13246,15 +13887,19 @@
       <c r="R69" s="201"/>
       <c r="S69" s="12"/>
       <c r="T69" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U69" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:22" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W69" s="219" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="192" t="s">
         <v>187</v>
       </c>
@@ -13268,7 +13913,7 @@
         <v>34</v>
       </c>
       <c r="E70" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="F70" s="196" t="s">
@@ -13304,15 +13949,19 @@
       <c r="R70" s="201"/>
       <c r="S70" s="12"/>
       <c r="T70" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U70" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:22" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W70" s="219" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="192" t="s">
         <v>187</v>
       </c>
@@ -13326,7 +13975,7 @@
         <v>34</v>
       </c>
       <c r="E71" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="F71" s="196" t="s">
@@ -13362,15 +14011,19 @@
       <c r="R71" s="201"/>
       <c r="S71" s="12"/>
       <c r="T71" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U71" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:22" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W71" s="219" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="192" t="s">
         <v>187</v>
       </c>
@@ -13384,7 +14037,7 @@
         <v>34</v>
       </c>
       <c r="E72" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.6</v>
       </c>
       <c r="F72" s="196" t="s">
@@ -13420,15 +14073,19 @@
       <c r="R72" s="201"/>
       <c r="S72" s="12"/>
       <c r="T72" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U72" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:22" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W72" s="219" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="192" t="s">
         <v>187</v>
       </c>
@@ -13442,7 +14099,7 @@
         <v>34</v>
       </c>
       <c r="E73" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.6</v>
       </c>
       <c r="F73" s="196" t="s">
@@ -13478,15 +14135,19 @@
       <c r="R73" s="201"/>
       <c r="S73" s="12"/>
       <c r="T73" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U73" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:22" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W73" s="219" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="192" t="s">
         <v>187</v>
       </c>
@@ -13500,7 +14161,7 @@
         <v>608</v>
       </c>
       <c r="E74" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.4905660377358486E-2</v>
       </c>
       <c r="F74" s="196" t="s">
@@ -13536,15 +14197,19 @@
       <c r="R74" s="201"/>
       <c r="S74" s="12"/>
       <c r="T74" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U74" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:22" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W74" s="219" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="192" t="s">
         <v>187</v>
       </c>
@@ -13558,7 +14223,7 @@
         <v>612</v>
       </c>
       <c r="E75" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.12600536193029491</v>
       </c>
       <c r="F75" s="196" t="s">
@@ -13594,15 +14259,19 @@
       <c r="R75" s="201"/>
       <c r="S75" s="12"/>
       <c r="T75" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U75" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:22" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W75" s="219" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="192" t="s">
         <v>187</v>
       </c>
@@ -13616,7 +14285,7 @@
         <v>34</v>
       </c>
       <c r="E76" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.6</v>
       </c>
       <c r="F76" s="196" t="s">
@@ -13652,15 +14321,19 @@
       <c r="R76" s="201"/>
       <c r="S76" s="12"/>
       <c r="T76" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U76" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:22" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W76" s="219" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="192" t="s">
         <v>187</v>
       </c>
@@ -13674,7 +14347,7 @@
         <v>34</v>
       </c>
       <c r="E77" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.6</v>
       </c>
       <c r="F77" s="196" t="s">
@@ -13710,15 +14383,19 @@
       <c r="R77" s="201"/>
       <c r="S77" s="12"/>
       <c r="T77" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U77" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:22" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W77" s="219" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="192" t="s">
         <v>19</v>
       </c>
@@ -13732,7 +14409,7 @@
         <v>34</v>
       </c>
       <c r="E78" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.65517241379310343</v>
       </c>
       <c r="F78" s="196" t="s">
@@ -13770,15 +14447,19 @@
       <c r="R78" s="201"/>
       <c r="S78" s="12"/>
       <c r="T78" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U78" s="195">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:22" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W78" s="219" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="192" t="s">
         <v>187</v>
       </c>
@@ -13792,7 +14473,7 @@
         <v>34</v>
       </c>
       <c r="E79" s="195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="F79" s="196" t="s">
@@ -13828,502 +14509,562 @@
       <c r="R79" s="201"/>
       <c r="S79" s="12"/>
       <c r="T79" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="U79" s="195">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="W79" s="219" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A80" s="138" t="s">
+        <v>187</v>
+      </c>
+      <c r="B80" s="138" t="s">
+        <v>373</v>
+      </c>
+      <c r="C80" s="139">
+        <v>100</v>
+      </c>
+      <c r="D80" s="151">
+        <v>120</v>
+      </c>
+      <c r="E80" s="140">
+        <f t="shared" ref="E80" si="12">SUM(D80-C80)/C80*100%</f>
+        <v>0.2</v>
+      </c>
+      <c r="F80" s="141" t="s">
+        <v>22</v>
+      </c>
+      <c r="G80" s="142" t="s">
+        <v>374</v>
+      </c>
+      <c r="H80" s="143" t="s">
+        <v>375</v>
+      </c>
+      <c r="I80" s="144" t="s">
+        <v>376</v>
+      </c>
+      <c r="J80" s="145">
+        <v>10971</v>
+      </c>
+      <c r="K80" s="146">
+        <v>43899</v>
+      </c>
+      <c r="L80" s="146">
+        <v>43901</v>
+      </c>
+      <c r="M80" s="142" t="s">
+        <v>26</v>
+      </c>
+      <c r="N80" s="147" t="s">
+        <v>377</v>
+      </c>
+      <c r="O80" s="147" t="s">
+        <v>377</v>
+      </c>
+      <c r="P80" s="144" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q80" s="144" t="s">
+        <v>378</v>
+      </c>
+      <c r="R80" s="148" t="s">
+        <v>58</v>
+      </c>
+      <c r="S80" s="149" t="s">
+        <v>241</v>
+      </c>
+      <c r="T80" s="140">
+        <f t="shared" si="9"/>
+        <v>-0.18</v>
+      </c>
+      <c r="U80" s="140">
+        <f t="shared" si="10"/>
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="V80" s="53" t="s">
+        <v>242</v>
+      </c>
+      <c r="W80" s="219">
+        <f t="shared" si="11"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="192" t="s">
+        <v>52</v>
+      </c>
+      <c r="B81" s="192" t="s">
+        <v>379</v>
+      </c>
+      <c r="C81" s="193" t="s">
+        <v>623</v>
+      </c>
+      <c r="D81" s="194" t="s">
+        <v>468</v>
+      </c>
+      <c r="E81" s="195">
+        <f t="shared" si="6"/>
+        <v>0.95918367346938771</v>
+      </c>
+      <c r="F81" s="196" t="s">
+        <v>35</v>
+      </c>
+      <c r="G81" s="197" t="s">
+        <v>374</v>
+      </c>
+      <c r="H81" s="198" t="s">
+        <v>44</v>
+      </c>
+      <c r="I81" s="194" t="s">
+        <v>380</v>
+      </c>
+      <c r="J81" s="199">
+        <v>661.05</v>
+      </c>
+      <c r="K81" s="200">
+        <v>44000</v>
+      </c>
+      <c r="L81" s="200">
+        <v>44001</v>
+      </c>
+      <c r="M81" s="197" t="s">
+        <v>26</v>
+      </c>
+      <c r="N81" s="191" t="s">
+        <v>624</v>
+      </c>
+      <c r="O81" s="191" t="s">
+        <v>624</v>
+      </c>
+      <c r="P81" s="194" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q81" s="194" t="s">
+        <v>625</v>
+      </c>
+      <c r="R81" s="201" t="s">
+        <v>491</v>
+      </c>
+      <c r="S81" s="194" t="s">
+        <v>464</v>
+      </c>
+      <c r="T81" s="195">
+        <f t="shared" si="9"/>
+        <v>6.1224489795918366E-2</v>
+      </c>
+      <c r="U81" s="195">
+        <f t="shared" si="10"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="W81" s="219">
+        <f t="shared" si="11"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="192" t="s">
+        <v>52</v>
+      </c>
+      <c r="B82" s="192" t="s">
+        <v>381</v>
+      </c>
+      <c r="C82" s="193" t="s">
+        <v>626</v>
+      </c>
+      <c r="D82" s="194" t="s">
+        <v>483</v>
+      </c>
+      <c r="E82" s="195">
+        <f t="shared" si="6"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="F82" s="197" t="s">
+        <v>22</v>
+      </c>
+      <c r="G82" s="197" t="s">
+        <v>374</v>
+      </c>
+      <c r="H82" s="198" t="s">
+        <v>44</v>
+      </c>
+      <c r="I82" s="194" t="s">
+        <v>382</v>
+      </c>
+      <c r="J82" s="203">
+        <v>4295.25</v>
+      </c>
+      <c r="K82" s="200">
+        <v>43997</v>
+      </c>
+      <c r="L82" s="200">
+        <v>43997</v>
+      </c>
+      <c r="M82" s="197" t="s">
+        <v>26</v>
+      </c>
+      <c r="N82" s="194" t="s">
+        <v>627</v>
+      </c>
+      <c r="O82" s="194" t="s">
+        <v>628</v>
+      </c>
+      <c r="P82" s="204" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q82" s="194" t="s">
+        <v>629</v>
+      </c>
+      <c r="R82" s="201">
+        <v>44096</v>
+      </c>
+      <c r="S82" s="194" t="s">
+        <v>476</v>
+      </c>
+      <c r="T82" s="195">
+        <f t="shared" si="9"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="U82" s="195">
+        <f t="shared" si="10"/>
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="W82" s="219">
+        <f t="shared" si="11"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="192" t="s">
+        <v>52</v>
+      </c>
+      <c r="B83" s="192" t="s">
+        <v>383</v>
+      </c>
+      <c r="C83" s="193" t="s">
+        <v>136</v>
+      </c>
+      <c r="D83" s="194" t="s">
+        <v>34</v>
+      </c>
+      <c r="E83" s="195">
+        <f t="shared" si="6"/>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="F83" s="197" t="s">
+        <v>68</v>
+      </c>
+      <c r="G83" s="197" t="s">
+        <v>374</v>
+      </c>
+      <c r="H83" s="198" t="s">
+        <v>44</v>
+      </c>
+      <c r="I83" s="194" t="s">
+        <v>384</v>
+      </c>
+      <c r="J83" s="203">
+        <v>1357.65</v>
+      </c>
+      <c r="K83" s="200">
+        <v>44027</v>
+      </c>
+      <c r="L83" s="200">
+        <v>44033</v>
+      </c>
+      <c r="M83" s="197" t="s">
+        <v>38</v>
+      </c>
+      <c r="N83" s="194" t="s">
+        <v>630</v>
+      </c>
+      <c r="O83" s="194" t="s">
+        <v>631</v>
+      </c>
+      <c r="P83" s="204" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q83" s="194" t="s">
+        <v>632</v>
+      </c>
+      <c r="R83" s="201">
+        <v>44096</v>
+      </c>
+      <c r="S83" s="194" t="s">
+        <v>499</v>
+      </c>
+      <c r="T83" s="195">
+        <f t="shared" si="9"/>
+        <v>0.15789473684210525</v>
+      </c>
+      <c r="U83" s="195">
+        <f t="shared" si="10"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="W83" s="219">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="192" t="s">
+        <v>52</v>
+      </c>
+      <c r="B84" s="192" t="s">
+        <v>385</v>
+      </c>
+      <c r="C84" s="193" t="s">
+        <v>633</v>
+      </c>
+      <c r="D84" s="194" t="s">
+        <v>499</v>
+      </c>
+      <c r="E84" s="195">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F84" s="197" t="s">
+        <v>68</v>
+      </c>
+      <c r="G84" s="197" t="s">
+        <v>374</v>
+      </c>
+      <c r="H84" s="198" t="s">
+        <v>44</v>
+      </c>
+      <c r="I84" s="194" t="s">
+        <v>386</v>
+      </c>
+      <c r="J84" s="203">
+        <v>1265.25</v>
+      </c>
+      <c r="K84" s="200">
+        <v>44027</v>
+      </c>
+      <c r="L84" s="200">
+        <v>44029</v>
+      </c>
+      <c r="M84" s="197" t="s">
+        <v>26</v>
+      </c>
+      <c r="N84" s="194" t="s">
+        <v>634</v>
+      </c>
+      <c r="O84" s="194" t="s">
+        <v>635</v>
+      </c>
+      <c r="P84" s="204" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q84" s="194" t="s">
+        <v>636</v>
+      </c>
+      <c r="R84" s="201">
+        <v>44096</v>
+      </c>
+      <c r="S84" s="194" t="s">
+        <v>470</v>
+      </c>
+      <c r="T84" s="195">
+        <f t="shared" si="9"/>
+        <v>0.21212121212121213</v>
+      </c>
+      <c r="U84" s="195">
+        <f t="shared" si="10"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="W84" s="219">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="192" t="s">
+        <v>52</v>
+      </c>
+      <c r="B85" s="192" t="s">
+        <v>387</v>
+      </c>
+      <c r="C85" s="193" t="s">
+        <v>633</v>
+      </c>
+      <c r="D85" s="194" t="s">
+        <v>476</v>
+      </c>
+      <c r="E85" s="195">
+        <f t="shared" si="6"/>
+        <v>1.1818181818181819</v>
+      </c>
+      <c r="F85" s="197" t="s">
+        <v>68</v>
+      </c>
+      <c r="G85" s="197" t="s">
+        <v>374</v>
+      </c>
+      <c r="H85" s="198" t="s">
+        <v>44</v>
+      </c>
+      <c r="I85" s="194" t="s">
+        <v>388</v>
+      </c>
+      <c r="J85" s="203">
+        <v>1450.05</v>
+      </c>
+      <c r="K85" s="200">
+        <v>44033</v>
+      </c>
+      <c r="L85" s="200">
+        <v>44034</v>
+      </c>
+      <c r="M85" s="197" t="s">
+        <v>38</v>
+      </c>
+      <c r="N85" s="194" t="s">
+        <v>637</v>
+      </c>
+      <c r="O85" s="194" t="s">
+        <v>638</v>
+      </c>
+      <c r="P85" s="194" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q85" s="194" t="s">
+        <v>639</v>
+      </c>
+      <c r="R85" s="201">
+        <v>44096</v>
+      </c>
+      <c r="S85" s="194" t="s">
+        <v>34</v>
+      </c>
+      <c r="T85" s="195">
+        <f t="shared" si="9"/>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="U85" s="195">
+        <f t="shared" si="10"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="W85" s="219">
+        <f t="shared" si="11"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="192" t="s">
+        <v>52</v>
+      </c>
+      <c r="B86" s="192" t="s">
+        <v>640</v>
+      </c>
+      <c r="C86" s="194" t="s">
+        <v>641</v>
+      </c>
+      <c r="D86" s="194" t="s">
+        <v>76</v>
+      </c>
+      <c r="E86" s="195">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="F86" s="197" t="s">
+        <v>68</v>
+      </c>
+      <c r="G86" s="197" t="s">
+        <v>374</v>
+      </c>
+      <c r="H86" s="198" t="s">
+        <v>44</v>
+      </c>
+      <c r="I86" s="194" t="s">
+        <v>642</v>
+      </c>
+      <c r="J86" s="203">
+        <v>895.65</v>
+      </c>
+      <c r="K86" s="200">
+        <v>44055</v>
+      </c>
+      <c r="L86" s="200">
+        <v>44056</v>
+      </c>
+      <c r="M86" s="197" t="s">
+        <v>26</v>
+      </c>
+      <c r="N86" s="194" t="s">
+        <v>643</v>
+      </c>
+      <c r="O86" s="194" t="s">
+        <v>644</v>
+      </c>
+      <c r="P86" s="194" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q86" s="194" t="s">
+        <v>645</v>
+      </c>
+      <c r="R86" s="201">
+        <v>44096</v>
+      </c>
+      <c r="S86" s="194" t="s">
+        <v>76</v>
+      </c>
+      <c r="T86" s="195">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" s="138" t="s">
-        <v>187</v>
-      </c>
-      <c r="B80" s="138" t="s">
-        <v>373</v>
-      </c>
-      <c r="C80" s="139">
-        <v>100</v>
-      </c>
-      <c r="D80" s="151">
-        <v>120</v>
-      </c>
-      <c r="E80" s="140">
-        <f t="shared" ref="E80" si="10">SUM(D80-C80)/C80*100%</f>
-        <v>0.2</v>
-      </c>
-      <c r="F80" s="141" t="s">
-        <v>22</v>
-      </c>
-      <c r="G80" s="142" t="s">
-        <v>374</v>
-      </c>
-      <c r="H80" s="143" t="s">
-        <v>375</v>
-      </c>
-      <c r="I80" s="144" t="s">
-        <v>376</v>
-      </c>
-      <c r="J80" s="145">
-        <v>10971</v>
-      </c>
-      <c r="K80" s="146">
-        <v>43899</v>
-      </c>
-      <c r="L80" s="146">
-        <v>43901</v>
-      </c>
-      <c r="M80" s="142" t="s">
-        <v>26</v>
-      </c>
-      <c r="N80" s="147" t="s">
-        <v>377</v>
-      </c>
-      <c r="O80" s="147" t="s">
-        <v>377</v>
-      </c>
-      <c r="P80" s="144" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q80" s="144" t="s">
-        <v>378</v>
-      </c>
-      <c r="R80" s="148" t="s">
-        <v>58</v>
-      </c>
-      <c r="S80" s="149" t="s">
-        <v>241</v>
-      </c>
-      <c r="T80" s="140">
-        <f t="shared" si="8"/>
-        <v>-0.18</v>
-      </c>
-      <c r="U80" s="140">
-        <f t="shared" si="9"/>
-        <v>0.31666666666666665</v>
-      </c>
-      <c r="V80" s="53" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="81" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="192" t="s">
-        <v>52</v>
-      </c>
-      <c r="B81" s="192" t="s">
-        <v>379</v>
-      </c>
-      <c r="C81" s="193" t="s">
-        <v>623</v>
-      </c>
-      <c r="D81" s="194" t="s">
-        <v>468</v>
-      </c>
-      <c r="E81" s="195">
-        <f t="shared" si="5"/>
-        <v>0.95918367346938771</v>
-      </c>
-      <c r="F81" s="196" t="s">
-        <v>35</v>
-      </c>
-      <c r="G81" s="197" t="s">
-        <v>374</v>
-      </c>
-      <c r="H81" s="198" t="s">
-        <v>44</v>
-      </c>
-      <c r="I81" s="194" t="s">
-        <v>380</v>
-      </c>
-      <c r="J81" s="199">
-        <v>661.05</v>
-      </c>
-      <c r="K81" s="200">
-        <v>44000</v>
-      </c>
-      <c r="L81" s="200">
-        <v>44001</v>
-      </c>
-      <c r="M81" s="197" t="s">
-        <v>26</v>
-      </c>
-      <c r="N81" s="191" t="s">
-        <v>624</v>
-      </c>
-      <c r="O81" s="191" t="s">
-        <v>624</v>
-      </c>
-      <c r="P81" s="194" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q81" s="194" t="s">
-        <v>625</v>
-      </c>
-      <c r="R81" s="201" t="s">
-        <v>491</v>
-      </c>
-      <c r="S81" s="194" t="s">
-        <v>464</v>
-      </c>
-      <c r="T81" s="195">
-        <f t="shared" si="8"/>
-        <v>6.1224489795918366E-2</v>
-      </c>
-      <c r="U81" s="195">
-        <f t="shared" si="9"/>
-        <v>0.45833333333333331</v>
-      </c>
-    </row>
-    <row r="82" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="192" t="s">
-        <v>52</v>
-      </c>
-      <c r="B82" s="192" t="s">
-        <v>381</v>
-      </c>
-      <c r="C82" s="193" t="s">
-        <v>626</v>
-      </c>
-      <c r="D82" s="194" t="s">
-        <v>483</v>
-      </c>
-      <c r="E82" s="195">
-        <f t="shared" si="5"/>
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="F82" s="197" t="s">
-        <v>22</v>
-      </c>
-      <c r="G82" s="197" t="s">
-        <v>374</v>
-      </c>
-      <c r="H82" s="198" t="s">
-        <v>44</v>
-      </c>
-      <c r="I82" s="194" t="s">
-        <v>382</v>
-      </c>
-      <c r="J82" s="203">
-        <v>4295.25</v>
-      </c>
-      <c r="K82" s="200">
-        <v>43997</v>
-      </c>
-      <c r="L82" s="200">
-        <v>43997</v>
-      </c>
-      <c r="M82" s="197" t="s">
-        <v>26</v>
-      </c>
-      <c r="N82" s="194" t="s">
-        <v>627</v>
-      </c>
-      <c r="O82" s="194" t="s">
-        <v>628</v>
-      </c>
-      <c r="P82" s="204" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q82" s="194" t="s">
-        <v>629</v>
-      </c>
-      <c r="R82" s="201">
-        <v>44096</v>
-      </c>
-      <c r="S82" s="194" t="s">
-        <v>476</v>
-      </c>
-      <c r="T82" s="195">
-        <f t="shared" si="8"/>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="U82" s="195">
-        <f t="shared" si="9"/>
-        <v>0.30769230769230771</v>
-      </c>
-    </row>
-    <row r="83" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="192" t="s">
-        <v>52</v>
-      </c>
-      <c r="B83" s="192" t="s">
-        <v>383</v>
-      </c>
-      <c r="C83" s="193" t="s">
-        <v>136</v>
-      </c>
-      <c r="D83" s="194" t="s">
-        <v>34</v>
-      </c>
-      <c r="E83" s="195">
-        <f t="shared" si="5"/>
-        <v>0.26315789473684209</v>
-      </c>
-      <c r="F83" s="197" t="s">
-        <v>68</v>
-      </c>
-      <c r="G83" s="197" t="s">
-        <v>374</v>
-      </c>
-      <c r="H83" s="198" t="s">
-        <v>44</v>
-      </c>
-      <c r="I83" s="194" t="s">
-        <v>384</v>
-      </c>
-      <c r="J83" s="203">
-        <v>1357.65</v>
-      </c>
-      <c r="K83" s="200">
-        <v>44027</v>
-      </c>
-      <c r="L83" s="200">
-        <v>44033</v>
-      </c>
-      <c r="M83" s="197" t="s">
-        <v>38</v>
-      </c>
-      <c r="N83" s="194" t="s">
-        <v>630</v>
-      </c>
-      <c r="O83" s="194" t="s">
-        <v>631</v>
-      </c>
-      <c r="P83" s="204" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q83" s="194" t="s">
-        <v>632</v>
-      </c>
-      <c r="R83" s="201">
-        <v>44096</v>
-      </c>
-      <c r="S83" s="194" t="s">
-        <v>499</v>
-      </c>
-      <c r="T83" s="195">
-        <f t="shared" si="8"/>
-        <v>0.15789473684210525</v>
-      </c>
-      <c r="U83" s="195">
-        <f t="shared" si="9"/>
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="192" t="s">
-        <v>52</v>
-      </c>
-      <c r="B84" s="192" t="s">
-        <v>385</v>
-      </c>
-      <c r="C84" s="193" t="s">
-        <v>633</v>
-      </c>
-      <c r="D84" s="194" t="s">
-        <v>499</v>
-      </c>
-      <c r="E84" s="195">
-        <f t="shared" si="5"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F84" s="197" t="s">
-        <v>68</v>
-      </c>
-      <c r="G84" s="197" t="s">
-        <v>374</v>
-      </c>
-      <c r="H84" s="198" t="s">
-        <v>44</v>
-      </c>
-      <c r="I84" s="194" t="s">
-        <v>386</v>
-      </c>
-      <c r="J84" s="203">
-        <v>1265.25</v>
-      </c>
-      <c r="K84" s="200">
-        <v>44027</v>
-      </c>
-      <c r="L84" s="200">
-        <v>44029</v>
-      </c>
-      <c r="M84" s="197" t="s">
-        <v>26</v>
-      </c>
-      <c r="N84" s="194" t="s">
-        <v>634</v>
-      </c>
-      <c r="O84" s="194" t="s">
-        <v>635</v>
-      </c>
-      <c r="P84" s="204" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q84" s="194" t="s">
-        <v>636</v>
-      </c>
-      <c r="R84" s="201">
-        <v>44096</v>
-      </c>
-      <c r="S84" s="194" t="s">
-        <v>470</v>
-      </c>
-      <c r="T84" s="195">
-        <f t="shared" si="8"/>
-        <v>0.21212121212121213</v>
-      </c>
-      <c r="U84" s="195">
-        <f t="shared" si="9"/>
-        <v>9.0909090909090912E-2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="192" t="s">
-        <v>52</v>
-      </c>
-      <c r="B85" s="192" t="s">
-        <v>387</v>
-      </c>
-      <c r="C85" s="193" t="s">
-        <v>633</v>
-      </c>
-      <c r="D85" s="194" t="s">
-        <v>476</v>
-      </c>
-      <c r="E85" s="195">
-        <f t="shared" si="5"/>
-        <v>1.1818181818181819</v>
-      </c>
-      <c r="F85" s="197" t="s">
-        <v>68</v>
-      </c>
-      <c r="G85" s="197" t="s">
-        <v>374</v>
-      </c>
-      <c r="H85" s="198" t="s">
-        <v>44</v>
-      </c>
-      <c r="I85" s="194" t="s">
-        <v>388</v>
-      </c>
-      <c r="J85" s="203">
-        <v>1450.05</v>
-      </c>
-      <c r="K85" s="200">
-        <v>44033</v>
-      </c>
-      <c r="L85" s="200">
-        <v>44034</v>
-      </c>
-      <c r="M85" s="197" t="s">
-        <v>38</v>
-      </c>
-      <c r="N85" s="194" t="s">
-        <v>637</v>
-      </c>
-      <c r="O85" s="194" t="s">
-        <v>638</v>
-      </c>
-      <c r="P85" s="194" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q85" s="194" t="s">
-        <v>639</v>
-      </c>
-      <c r="R85" s="201">
-        <v>44096</v>
-      </c>
-      <c r="S85" s="194" t="s">
-        <v>34</v>
-      </c>
-      <c r="T85" s="195">
-        <f t="shared" si="8"/>
-        <v>0.45454545454545453</v>
-      </c>
-      <c r="U85" s="195">
-        <f t="shared" si="9"/>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="86" spans="1:21" s="209" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="192" t="s">
-        <v>52</v>
-      </c>
-      <c r="B86" s="192" t="s">
-        <v>640</v>
-      </c>
-      <c r="C86" s="194" t="s">
-        <v>641</v>
-      </c>
-      <c r="D86" s="194" t="s">
-        <v>76</v>
-      </c>
-      <c r="E86" s="195">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="F86" s="197" t="s">
-        <v>68</v>
-      </c>
-      <c r="G86" s="197" t="s">
-        <v>374</v>
-      </c>
-      <c r="H86" s="198" t="s">
-        <v>44</v>
-      </c>
-      <c r="I86" s="194" t="s">
-        <v>642</v>
-      </c>
-      <c r="J86" s="203">
-        <v>895.65</v>
-      </c>
-      <c r="K86" s="200">
-        <v>44055</v>
-      </c>
-      <c r="L86" s="200">
-        <v>44056</v>
-      </c>
-      <c r="M86" s="197" t="s">
-        <v>26</v>
-      </c>
-      <c r="N86" s="194" t="s">
-        <v>643</v>
-      </c>
-      <c r="O86" s="194" t="s">
-        <v>644</v>
-      </c>
-      <c r="P86" s="194" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q86" s="194" t="s">
-        <v>645</v>
-      </c>
-      <c r="R86" s="201">
-        <v>44096</v>
-      </c>
-      <c r="S86" s="194" t="s">
-        <v>76</v>
-      </c>
-      <c r="T86" s="195">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="U86" s="195">
-        <f t="shared" si="9"/>
+      <c r="U86" s="221">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="W86" s="219">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U87" s="222" t="s">
+        <v>647</v>
+      </c>
+      <c r="V87" s="223"/>
+      <c r="W87" s="224">
+        <f>SUMSQ(W2:W86)</f>
+        <v>21037</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U88" s="222" t="s">
+        <v>648</v>
+      </c>
+      <c r="V88" s="223"/>
+      <c r="W88" s="224">
+        <f>COUNT(W2:W86)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="89" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="E89" s="66" t="s">
         <v>390</v>
       </c>
-      <c r="T89" s="66" t="s">
+      <c r="T89" s="220" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U89" s="225" t="s">
+        <v>649</v>
+      </c>
+      <c r="V89" s="223"/>
+      <c r="W89" s="226">
+        <f>SQRT(W87/W88)</f>
+        <v>18.724760790639401</v>
+      </c>
+    </row>
+    <row r="90" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C90" s="217" t="s">
         <v>389</v>
       </c>
@@ -14351,12 +15092,8 @@
         <f>AVERAGE(T2:T86)</f>
         <v>-2.5663455831541396E-2</v>
       </c>
-      <c r="U90" s="56">
-        <f>AVERAGE(U2:U80)</f>
-        <v>0.44015746447583604</v>
-      </c>
-    </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C91" s="217" t="s">
         <v>391</v>
       </c>
@@ -14385,7 +15122,7 @@
         <v>-5.3498640060256349E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C92" s="217" t="s">
         <v>392</v>
       </c>
@@ -14414,7 +15151,7 @@
         <v>0.28450002557413939</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
implementando rotinas para inserir aruivo para teste de deploy
</commit_message>
<xml_diff>
--- a/dados/Exercicio_estimativa_de_paginas_2019_2020_joas_novo.xlsx
+++ b/dados/Exercicio_estimativa_de_paginas_2019_2020_joas_novo.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wpessoa/repositorios/Fluxo_Editorial/dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4869808D-BE5B-614B-9092-9B3047EFA563}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930D3B8D-C1D9-B548-988C-7D11218B337F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3460" yWindow="580" windowWidth="29040" windowHeight="16440" xr2:uid="{65A40DB1-9662-402A-9A88-8271FB79FF7C}"/>
+    <workbookView xWindow="2920" yWindow="2260" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{65A40DB1-9662-402A-9A88-8271FB79FF7C}"/>
   </bookViews>
   <sheets>
     <sheet name="EXECUTADO 2019" sheetId="4" r:id="rId1"/>
@@ -3445,10 +3445,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B51CFDF2-E479-4AF3-B196-4948E99A1239}">
-  <dimension ref="A1:W78"/>
+  <sheetPr codeName="Planilha1"/>
+  <dimension ref="A1:W92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="W73" sqref="W73"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F70" sqref="F2:F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3470,8 +3471,8 @@
     <col min="17" max="17" width="9" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="12.5" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="9" customWidth="1"/>
-    <col min="20" max="20" width="20.5" customWidth="1"/>
-    <col min="21" max="21" width="23.33203125" customWidth="1"/>
+    <col min="20" max="20" width="20.5" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="23.33203125" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="109.1640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8722,7 +8723,7 @@
       </c>
     </row>
     <row r="71" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="U71" s="222" t="s">
+      <c r="G71" s="222" t="s">
         <v>647</v>
       </c>
       <c r="V71" s="223"/>
@@ -8732,7 +8733,7 @@
       </c>
     </row>
     <row r="72" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="U72" s="222" t="s">
+      <c r="G72" s="222" t="s">
         <v>648</v>
       </c>
       <c r="V72" s="223"/>
@@ -8741,14 +8742,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:23" ht="16" x14ac:dyDescent="0.2">
-      <c r="E73" s="66" t="s">
-        <v>390</v>
-      </c>
-      <c r="T73" s="66" t="s">
-        <v>390</v>
-      </c>
-      <c r="U73" s="225" t="s">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="G73" s="225" t="s">
         <v>649</v>
       </c>
       <c r="V73" s="223"/>
@@ -8758,109 +8753,116 @@
       </c>
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C74" s="217" t="s">
-        <v>389</v>
-      </c>
-      <c r="D74" s="217"/>
-      <c r="E74" s="68">
-        <f>AVERAGE(E2:E70)</f>
-        <v>0.57629739780999889</v>
-      </c>
-      <c r="G74" s="217" t="s">
-        <v>389</v>
-      </c>
-      <c r="H74" s="217"/>
-      <c r="I74" s="217"/>
-      <c r="J74" s="217"/>
-      <c r="K74" s="217"/>
-      <c r="L74" s="217"/>
-      <c r="M74" s="217"/>
-      <c r="N74" s="217"/>
-      <c r="O74" s="217"/>
-      <c r="P74" s="217"/>
-      <c r="Q74" s="217"/>
-      <c r="R74" s="217"/>
-      <c r="S74" s="217"/>
-      <c r="T74" s="68">
-        <f ca="1">AVERAGE(T2:T70)</f>
-        <v>0.35225423922134153</v>
-      </c>
-      <c r="U74" s="56">
-        <f>AVERAGE(U2:U70)</f>
-        <v>0.1334030966806202</v>
-      </c>
-    </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C75" s="217" t="s">
-        <v>391</v>
-      </c>
-      <c r="D75" s="217"/>
-      <c r="E75" s="69">
-        <f>AVERAGE(E2:E67)</f>
-        <v>0.59654720281210283</v>
-      </c>
-      <c r="G75" s="217" t="s">
-        <v>391</v>
-      </c>
-      <c r="H75" s="217"/>
-      <c r="I75" s="217"/>
-      <c r="J75" s="217"/>
-      <c r="K75" s="217"/>
-      <c r="L75" s="217"/>
-      <c r="M75" s="217"/>
-      <c r="N75" s="217"/>
-      <c r="O75" s="217"/>
-      <c r="P75" s="217"/>
-      <c r="Q75" s="217"/>
-      <c r="R75" s="217"/>
-      <c r="S75" s="217"/>
-      <c r="T75" s="68">
-        <f>AVERAGE(T2:T67)</f>
-        <v>0.36922475220474349</v>
-      </c>
-    </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C76" s="217" t="s">
-        <v>392</v>
-      </c>
-      <c r="D76" s="217"/>
-      <c r="E76" s="69">
-        <f>AVERAGE(E68:E70)</f>
-        <v>0.13080168776371306</v>
-      </c>
-      <c r="G76" s="217" t="s">
-        <v>392</v>
-      </c>
-      <c r="H76" s="217"/>
-      <c r="I76" s="217"/>
-      <c r="J76" s="217"/>
-      <c r="K76" s="217"/>
-      <c r="L76" s="217"/>
-      <c r="M76" s="217"/>
-      <c r="N76" s="217"/>
-      <c r="O76" s="217"/>
-      <c r="P76" s="217"/>
-      <c r="Q76" s="217"/>
-      <c r="R76" s="217"/>
-      <c r="S76" s="217"/>
-      <c r="T76" s="68">
-        <f ca="1">AVERAGE(T68:T70)</f>
-        <v>0</v>
-      </c>
+      <c r="G74" s="56"/>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C78" s="135"/>
       <c r="S78" s="135"/>
       <c r="T78" s="56"/>
     </row>
+    <row r="89" spans="3:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="E89" s="66" t="s">
+        <v>390</v>
+      </c>
+      <c r="T89" s="66" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="90" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C90" s="217" t="s">
+        <v>389</v>
+      </c>
+      <c r="D90" s="217"/>
+      <c r="E90" s="68">
+        <f>AVERAGE(E2:E70)</f>
+        <v>0.57629739780999889</v>
+      </c>
+      <c r="G90" s="217" t="s">
+        <v>389</v>
+      </c>
+      <c r="H90" s="217"/>
+      <c r="I90" s="217"/>
+      <c r="J90" s="217"/>
+      <c r="K90" s="217"/>
+      <c r="L90" s="217"/>
+      <c r="M90" s="217"/>
+      <c r="N90" s="217"/>
+      <c r="O90" s="217"/>
+      <c r="P90" s="217"/>
+      <c r="Q90" s="217"/>
+      <c r="R90" s="217"/>
+      <c r="S90" s="217"/>
+      <c r="T90" s="68">
+        <f ca="1">AVERAGE(T2:T70)</f>
+        <v>0.35225423922134153</v>
+      </c>
+    </row>
+    <row r="91" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C91" s="217" t="s">
+        <v>391</v>
+      </c>
+      <c r="D91" s="217"/>
+      <c r="E91" s="69">
+        <f>AVERAGE(E2:E67)</f>
+        <v>0.59654720281210283</v>
+      </c>
+      <c r="G91" s="217" t="s">
+        <v>391</v>
+      </c>
+      <c r="H91" s="217"/>
+      <c r="I91" s="217"/>
+      <c r="J91" s="217"/>
+      <c r="K91" s="217"/>
+      <c r="L91" s="217"/>
+      <c r="M91" s="217"/>
+      <c r="N91" s="217"/>
+      <c r="O91" s="217"/>
+      <c r="P91" s="217"/>
+      <c r="Q91" s="217"/>
+      <c r="R91" s="217"/>
+      <c r="S91" s="217"/>
+      <c r="T91" s="68">
+        <f>AVERAGE(T2:T67)</f>
+        <v>0.36922475220474349</v>
+      </c>
+    </row>
+    <row r="92" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C92" s="217" t="s">
+        <v>392</v>
+      </c>
+      <c r="D92" s="217"/>
+      <c r="E92" s="69">
+        <f>AVERAGE(E68:E70)</f>
+        <v>0.13080168776371306</v>
+      </c>
+      <c r="G92" s="217" t="s">
+        <v>392</v>
+      </c>
+      <c r="H92" s="217"/>
+      <c r="I92" s="217"/>
+      <c r="J92" s="217"/>
+      <c r="K92" s="217"/>
+      <c r="L92" s="217"/>
+      <c r="M92" s="217"/>
+      <c r="N92" s="217"/>
+      <c r="O92" s="217"/>
+      <c r="P92" s="217"/>
+      <c r="Q92" s="217"/>
+      <c r="R92" s="217"/>
+      <c r="S92" s="217"/>
+      <c r="T92" s="68">
+        <f ca="1">AVERAGE(T68:T70)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="G74:S74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="G75:S75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="G76:S76"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="G90:S90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="G91:S91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="G92:S92"/>
   </mergeCells>
   <conditionalFormatting sqref="T2:U2 T43:U67 T70:U70">
     <cfRule type="cellIs" dxfId="7" priority="5" operator="lessThan">
@@ -8888,10 +8890,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B00B66-C32D-4DEF-9BC0-D9C09304FF24}">
-  <dimension ref="A1:W94"/>
+  <sheetPr codeName="Planilha2"/>
+  <dimension ref="A1:W100"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="U87" sqref="U87:W89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I86" sqref="I2:I86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8913,8 +8916,8 @@
     <col min="17" max="17" width="9" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="12.5" customWidth="1"/>
     <col min="19" max="19" width="9" customWidth="1"/>
-    <col min="20" max="20" width="20.5" customWidth="1"/>
-    <col min="21" max="21" width="23.33203125" customWidth="1"/>
+    <col min="20" max="20" width="20.5" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="23.33203125" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="109.1640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -15028,8 +15031,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="U87" s="222" t="s">
+    <row r="87" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R87" s="222" t="s">
         <v>647</v>
       </c>
       <c r="V87" s="223"/>
@@ -15039,7 +15042,7 @@
       </c>
     </row>
     <row r="88" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="U88" s="222" t="s">
+      <c r="R88" s="222" t="s">
         <v>648</v>
       </c>
       <c r="V88" s="223"/>
@@ -15048,14 +15051,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="16" x14ac:dyDescent="0.2">
-      <c r="E89" s="66" t="s">
-        <v>390</v>
-      </c>
-      <c r="T89" s="220" t="s">
-        <v>390</v>
-      </c>
-      <c r="U89" s="225" t="s">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R89" s="225" t="s">
         <v>649</v>
       </c>
       <c r="V89" s="223"/>
@@ -15064,93 +15061,6 @@
         <v>18.724760790639401</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C90" s="217" t="s">
-        <v>389</v>
-      </c>
-      <c r="D90" s="217"/>
-      <c r="E90" s="68">
-        <f>AVERAGE(E2:E86)</f>
-        <v>0.69613300605749173</v>
-      </c>
-      <c r="G90" s="217" t="s">
-        <v>389</v>
-      </c>
-      <c r="H90" s="217"/>
-      <c r="I90" s="217"/>
-      <c r="J90" s="217"/>
-      <c r="K90" s="217"/>
-      <c r="L90" s="217"/>
-      <c r="M90" s="217"/>
-      <c r="N90" s="217"/>
-      <c r="O90" s="217"/>
-      <c r="P90" s="217"/>
-      <c r="Q90" s="217"/>
-      <c r="R90" s="217"/>
-      <c r="S90" s="217"/>
-      <c r="T90" s="68">
-        <f>AVERAGE(T2:T86)</f>
-        <v>-2.5663455831541396E-2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C91" s="217" t="s">
-        <v>391</v>
-      </c>
-      <c r="D91" s="217"/>
-      <c r="E91" s="69">
-        <f>AVERAGE(E2:E79)</f>
-        <v>0.69713678941520762</v>
-      </c>
-      <c r="G91" s="217" t="s">
-        <v>391</v>
-      </c>
-      <c r="H91" s="217"/>
-      <c r="I91" s="217"/>
-      <c r="J91" s="217"/>
-      <c r="K91" s="217"/>
-      <c r="L91" s="217"/>
-      <c r="M91" s="217"/>
-      <c r="N91" s="217"/>
-      <c r="O91" s="217"/>
-      <c r="P91" s="217"/>
-      <c r="Q91" s="217"/>
-      <c r="R91" s="217"/>
-      <c r="S91" s="217"/>
-      <c r="T91" s="68">
-        <f>AVERAGE(T2:T79)</f>
-        <v>-5.3498640060256349E-2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C92" s="217" t="s">
-        <v>392</v>
-      </c>
-      <c r="D92" s="217"/>
-      <c r="E92" s="69">
-        <f>AVERAGE(E80:E86)</f>
-        <v>0.68494799150008601</v>
-      </c>
-      <c r="G92" s="217" t="s">
-        <v>392</v>
-      </c>
-      <c r="H92" s="217"/>
-      <c r="I92" s="217"/>
-      <c r="J92" s="217"/>
-      <c r="K92" s="217"/>
-      <c r="L92" s="217"/>
-      <c r="M92" s="217"/>
-      <c r="N92" s="217"/>
-      <c r="O92" s="217"/>
-      <c r="P92" s="217"/>
-      <c r="Q92" s="217"/>
-      <c r="R92" s="217"/>
-      <c r="S92" s="217"/>
-      <c r="T92" s="68">
-        <f>AVERAGE(T80:T86)</f>
-        <v>0.28450002557413939</v>
-      </c>
-    </row>
     <row r="94" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>42</v>
@@ -15159,14 +15069,109 @@
       <c r="S94" s="135"/>
       <c r="T94" s="56"/>
     </row>
+    <row r="97" spans="3:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="E97" s="66" t="s">
+        <v>390</v>
+      </c>
+      <c r="T97" s="220" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="98" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C98" s="217" t="s">
+        <v>389</v>
+      </c>
+      <c r="D98" s="217"/>
+      <c r="E98" s="68">
+        <f>AVERAGE(E2:E86)</f>
+        <v>0.69613300605749173</v>
+      </c>
+      <c r="G98" s="217" t="s">
+        <v>389</v>
+      </c>
+      <c r="H98" s="217"/>
+      <c r="I98" s="217"/>
+      <c r="J98" s="217"/>
+      <c r="K98" s="217"/>
+      <c r="L98" s="217"/>
+      <c r="M98" s="217"/>
+      <c r="N98" s="217"/>
+      <c r="O98" s="217"/>
+      <c r="P98" s="217"/>
+      <c r="Q98" s="217"/>
+      <c r="R98" s="217"/>
+      <c r="S98" s="217"/>
+      <c r="T98" s="68">
+        <f>AVERAGE(T2:T86)</f>
+        <v>-2.5663455831541396E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C99" s="217" t="s">
+        <v>391</v>
+      </c>
+      <c r="D99" s="217"/>
+      <c r="E99" s="69">
+        <f>AVERAGE(E2:E79)</f>
+        <v>0.69713678941520762</v>
+      </c>
+      <c r="G99" s="217" t="s">
+        <v>391</v>
+      </c>
+      <c r="H99" s="217"/>
+      <c r="I99" s="217"/>
+      <c r="J99" s="217"/>
+      <c r="K99" s="217"/>
+      <c r="L99" s="217"/>
+      <c r="M99" s="217"/>
+      <c r="N99" s="217"/>
+      <c r="O99" s="217"/>
+      <c r="P99" s="217"/>
+      <c r="Q99" s="217"/>
+      <c r="R99" s="217"/>
+      <c r="S99" s="217"/>
+      <c r="T99" s="68">
+        <f>AVERAGE(T2:T79)</f>
+        <v>-5.3498640060256349E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C100" s="217" t="s">
+        <v>392</v>
+      </c>
+      <c r="D100" s="217"/>
+      <c r="E100" s="69">
+        <f>AVERAGE(E80:E86)</f>
+        <v>0.68494799150008601</v>
+      </c>
+      <c r="G100" s="217" t="s">
+        <v>392</v>
+      </c>
+      <c r="H100" s="217"/>
+      <c r="I100" s="217"/>
+      <c r="J100" s="217"/>
+      <c r="K100" s="217"/>
+      <c r="L100" s="217"/>
+      <c r="M100" s="217"/>
+      <c r="N100" s="217"/>
+      <c r="O100" s="217"/>
+      <c r="P100" s="217"/>
+      <c r="Q100" s="217"/>
+      <c r="R100" s="217"/>
+      <c r="S100" s="217"/>
+      <c r="T100" s="68">
+        <f>AVERAGE(T80:T86)</f>
+        <v>0.28450002557413939</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="G91:S91"/>
-    <mergeCell ref="G92:S92"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="G90:S90"/>
+    <mergeCell ref="G99:S99"/>
+    <mergeCell ref="G100:S100"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="G98:S98"/>
   </mergeCells>
   <conditionalFormatting sqref="T2:U41 T48:U86">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
@@ -15184,6 +15189,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C36815-82FF-4FD2-A1FA-43046145DAFC}">
+  <sheetPr codeName="Planilha3"/>
   <dimension ref="A1:V70"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
@@ -19445,6 +19451,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05DE1162-C7B1-41A4-A8B4-D8A5BE8EEEBA}">
+  <sheetPr codeName="Planilha4"/>
   <dimension ref="A1:V48"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">

</xml_diff>